<commit_message>
Aggiunto script per estrarre POI da TripAdvisor
</commit_message>
<xml_diff>
--- a/RASTA/risultati/NostriPOI/CTM/result_TD/topics.xlsx
+++ b/RASTA/risultati/NostriPOI/CTM/result_TD/topics.xlsx
@@ -468,156 +468,156 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>comune</t>
+          <t>meteorologico</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>territorio</t>
+          <t>coordinare</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>abitanti</t>
+          <t>trentennale</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>paese</t>
+          <t>geografico</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>comunale</t>
+          <t>coordinata</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>aquila</t>
+          <t>caldo</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>borgo</t>
+          <t>climatologico</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>località</t>
+          <t>lacerazione</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>dal</t>
+          <t>fabiano</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>nel</t>
+          <t>integrazione</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>servita</t>
+          <t>sala</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>torna</t>
+          <t>pinacoteca</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>contratto</t>
+          <t>transetto</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ferroviario</t>
+          <t>abside</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>interessata</t>
+          <t>attribuire</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>attesa</t>
+          <t>descrizione</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>geografiche</t>
+          <t>culturaitalia</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>trenitalia</t>
+          <t>sec</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ferroviari</t>
+          <t>dipinto</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>meteorologica</t>
+          <t>francescano</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cattolico</t>
+          <t>abitante</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>descrizione</t>
+          <t>situare</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>monofore</t>
+          <t>paese</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>fortunato</t>
+          <t>frazione</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>spoletium</t>
+          <t>castello</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>sorreggenti</t>
+          <t>località</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>web</t>
+          <t>strada</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>pedale</t>
+          <t>monte</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ospitata</t>
+          <t>geografia</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>illuminata</t>
+          <t>territorio</t>
         </is>
       </c>
     </row>
@@ -629,17 +629,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>naturale</t>
+          <t>flora</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>montuoso</t>
+          <t>idrografico</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>habitat</t>
+          <t>gettare</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -649,121 +649,121 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>boschi</t>
+          <t>cinghiale</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>appenninico</t>
+          <t>cresta</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>flora</t>
+          <t>cascata</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>orfento</t>
+          <t>profondità</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>specie</t>
+          <t>escursionistico</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>viabilità</t>
+          <t>fulvio</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>vocazione</t>
+          <t>censimento</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>cartaginese</t>
+          <t>corgna</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ceppo</t>
+          <t>sagra</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>aternum</t>
+          <t>toscana</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>peakbagger</t>
+          <t>mastioo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>galli</t>
+          <t>ascanio</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>enzo</t>
+          <t>cortona</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>valorizzare</t>
+          <t>anagno</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>coprono</t>
+          <t>rimuovere</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>stele</t>
+          <t>acerbo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>collezioni</t>
+          <t>lacuno</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ridotte</t>
+          <t>tessile</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>spoletium</t>
+          <t>interpretabile</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>beniculturali</t>
+          <t>calce</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>culturaitalia</t>
+          <t>alteravare</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>rinnovamento</t>
+          <t>gigante</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>cattolico</t>
+          <t>ciclopico</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -773,59 +773,59 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>stanze</t>
+          <t>indirizzare</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>chiesa</t>
+          <t>con</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>essere</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>madonna</t>
+          <t>che</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>uno</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>cui</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>trova</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>museo</t>
+          <t>per</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>santa</t>
+          <t>più</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>della</t>
+          <t>avere</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>nella</t>
+          <t>venire</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>nel</t>
+          <t>due</t>
         </is>
       </c>
     </row>

</xml_diff>